<commit_message>
feat(etl): bonus exercice 4 : top 3 pays par langues parlées
</commit_message>
<xml_diff>
--- a/etl/exercices/exercice4/pays_europe.xlsx
+++ b/etl/exercices/exercice4/pays_europe.xlsx
@@ -10,6 +10,7 @@
     <sheet name="pays_europe" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="population_top_5" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="plays_le_plus_densee" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="top_3_pays_langues_parless" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1824,4 +1825,79 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>population</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Russian</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>155137605</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Catalan</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>108331988</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>14</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>German</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>105240604</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>